<commit_message>
Reduce sleep time to 30 seconds in update_xl.py
Reduce the sleep time in the script to enahnce execution time since increased sleep time (60 seconds) does not resolve the issue of imprecise location
</commit_message>
<xml_diff>
--- a/data/cbus_trivia_list.xlsx
+++ b/data/cbus_trivia_list.xlsx
@@ -48,6 +48,11 @@
     <comment authorId="0" ref="V4">
       <text>
         <t xml:space="preserve">Just the 2nd Friday of each month</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="B6">
+      <text>
+        <t xml:space="preserve">Feud</t>
       </text>
     </comment>
     <comment authorId="0" ref="L6">
@@ -161,25 +166,25 @@
         <t xml:space="preserve">Musical Goodness</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L26">
-      <text>
-        <t xml:space="preserve">Sudden Songs</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="L27">
       <text>
         <t xml:space="preserve">Sudden Songs</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L36">
+    <comment authorId="0" ref="L28">
       <text>
-        <t xml:space="preserve">Name That Tune</t>
+        <t xml:space="preserve">Sudden Songs</t>
       </text>
     </comment>
     <comment authorId="0" ref="Q36">
       <text>
         <t xml:space="preserve">Music Trivia
 </t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="L37">
+      <text>
+        <t xml:space="preserve">Name That Tune</t>
       </text>
     </comment>
     <comment authorId="0" ref="Q40">
@@ -219,11 +224,6 @@
         <t xml:space="preserve">Music Trivia with Ric Knight</t>
       </text>
     </comment>
-    <comment authorId="0" ref="L55">
-      <text>
-        <t xml:space="preserve">"Trivia with Jason"</t>
-      </text>
-    </comment>
     <comment authorId="0" ref="G56">
       <text>
         <t xml:space="preserve">Blonde Vanity
@@ -231,6 +231,11 @@
       </text>
     </comment>
     <comment authorId="0" ref="L56">
+      <text>
+        <t xml:space="preserve">"Trivia with Jason"</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="L57">
       <text>
         <t xml:space="preserve">Music Trivia
 </t>
@@ -241,21 +246,15 @@
         <t xml:space="preserve">3rd Tuesday of each month</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K60">
+    <comment authorId="0" ref="K61">
       <text>
         <t xml:space="preserve">Hosted on the 2nd floor</t>
       </text>
     </comment>
-    <comment authorId="0" ref="K64">
+    <comment authorId="0" ref="K65">
       <text>
         <t xml:space="preserve">Different themed trivia each Wednesday 
 https://www.facebook.com/nocterrabrewing/upcoming_hosted_events</t>
-      </text>
-    </comment>
-    <comment authorId="0" ref="B6">
-      <text>
-        <t xml:space="preserve">Feud
-	-Robert Nolan</t>
       </text>
     </comment>
   </commentList>
@@ -263,7 +262,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="278">
   <si>
     <t>MONDAY</t>
   </si>
@@ -397,9 +396,6 @@
     <t>Dempsey's Food and Spirits</t>
   </si>
   <si>
-    <t>Jay</t>
-  </si>
-  <si>
     <t>Jackie O's On Fourth</t>
   </si>
   <si>
@@ -409,207 +405,204 @@
     <t>Lee's Sports and Spirits</t>
   </si>
   <si>
+    <t>Colin</t>
+  </si>
+  <si>
+    <t>Pastimes Crosswoods</t>
+  </si>
+  <si>
+    <t>Grizzlybird Brewing Company</t>
+  </si>
+  <si>
+    <t>Global Gallery</t>
+  </si>
+  <si>
+    <t>Chloe</t>
+  </si>
+  <si>
+    <t>Carfagna's</t>
+  </si>
+  <si>
+    <t>DJ Trivia</t>
+  </si>
+  <si>
+    <t>Porch Growler</t>
+  </si>
+  <si>
+    <t>Derek</t>
+  </si>
+  <si>
+    <t>Pastimes Grandview</t>
+  </si>
+  <si>
+    <t>Peter</t>
+  </si>
+  <si>
+    <t>https://excessstrivia.com/</t>
+  </si>
+  <si>
+    <t>Brewdog New Albany</t>
+  </si>
+  <si>
+    <t>Sweet Harmony Canal</t>
+  </si>
+  <si>
+    <t>World of Beer Easton</t>
+  </si>
+  <si>
+    <t>MC Boombox</t>
+  </si>
+  <si>
+    <t>Adobe Gila's</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>SATURDAY</t>
+  </si>
+  <si>
+    <t>Bryne's Pub</t>
+  </si>
+  <si>
+    <t>I Drink &amp; I Know</t>
+  </si>
+  <si>
+    <t>Alan</t>
+  </si>
+  <si>
+    <t>The Walrus</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>Aficianado's</t>
+  </si>
+  <si>
+    <t>Corey</t>
+  </si>
+  <si>
+    <t>Good Night John Boy</t>
+  </si>
+  <si>
+    <t>Chris</t>
+  </si>
+  <si>
+    <t>Barley Hopster's</t>
+  </si>
+  <si>
+    <t>DJ Rabbit</t>
+  </si>
+  <si>
+    <t>Keith</t>
+  </si>
+  <si>
+    <t>Trivia Goodness</t>
+  </si>
+  <si>
+    <t>Hey Hey Bar &amp; Grill</t>
+  </si>
+  <si>
+    <t>Pint and a Half</t>
+  </si>
+  <si>
+    <t>Zaftig Brewing Company</t>
+  </si>
+  <si>
+    <t>City Tavern Short North</t>
+  </si>
+  <si>
+    <t>Rini</t>
+  </si>
+  <si>
+    <t>Olentangy River Brewing</t>
+  </si>
+  <si>
+    <t>Jarvis</t>
+  </si>
+  <si>
+    <t>Gatsby's</t>
+  </si>
+  <si>
+    <t>CT Audio Productions</t>
+  </si>
+  <si>
+    <t>https://www.triviagoodness.com/play/</t>
+  </si>
+  <si>
+    <t>Keystone Pub &amp; Patio</t>
+  </si>
+  <si>
+    <t>Bada Bean Bada Booze</t>
+  </si>
+  <si>
+    <t>Ethyl &amp; Tank</t>
+  </si>
+  <si>
+    <t>Leiah</t>
+  </si>
+  <si>
+    <t>Park St Tavern</t>
+  </si>
+  <si>
+    <t>Blake</t>
+  </si>
+  <si>
+    <t>Traditions Tavern</t>
+  </si>
+  <si>
+    <t>Question Everything</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Bobcat Sports Bar</t>
+  </si>
+  <si>
+    <t>Baylee</t>
+  </si>
+  <si>
+    <t>Hanks Texas BBQ Clintonville</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Rule 3</t>
+  </si>
+  <si>
+    <t>The Draft Room</t>
+  </si>
+  <si>
+    <t>Big Head Trivia</t>
+  </si>
+  <si>
+    <t>Budd Dairy</t>
+  </si>
+  <si>
+    <t>Jac &amp; Do's on High</t>
+  </si>
+  <si>
+    <t>Slammers</t>
+  </si>
+  <si>
+    <t>Emaleigh</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/bigheadtrivia/</t>
+  </si>
+  <si>
+    <t>Google Map Links added for all Monday shows on 6/5/24</t>
+  </si>
+  <si>
+    <t>Fenders in Polaris</t>
+  </si>
+  <si>
     <t>Sarah</t>
   </si>
   <si>
-    <t>Pastimes Crosswoods</t>
-  </si>
-  <si>
-    <t>Colin</t>
-  </si>
-  <si>
-    <t>Grizzlybird Brewing Company</t>
-  </si>
-  <si>
-    <t>Global Gallery</t>
-  </si>
-  <si>
-    <t>Chloe</t>
-  </si>
-  <si>
-    <t>Carfagna's</t>
-  </si>
-  <si>
-    <t>DJ Trivia</t>
-  </si>
-  <si>
-    <t>Porch Growler</t>
-  </si>
-  <si>
-    <t>Derek</t>
-  </si>
-  <si>
-    <t>Pastimes Grandview</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>https://excessstrivia.com/</t>
-  </si>
-  <si>
-    <t>Brewdog New Albany</t>
-  </si>
-  <si>
-    <t>Sweet Harmony Canal</t>
-  </si>
-  <si>
-    <t>Sabrina</t>
-  </si>
-  <si>
-    <t>World of Beer Easton</t>
-  </si>
-  <si>
-    <t>Allyson</t>
-  </si>
-  <si>
-    <t>Adobe Gila's</t>
-  </si>
-  <si>
-    <t>Matthew</t>
-  </si>
-  <si>
-    <t>SATURDAY</t>
-  </si>
-  <si>
-    <t>Bryne's Pub</t>
-  </si>
-  <si>
-    <t>I Drink &amp; I Know</t>
-  </si>
-  <si>
-    <t>Alan</t>
-  </si>
-  <si>
-    <t>The Walrus</t>
-  </si>
-  <si>
-    <t>Spencer</t>
-  </si>
-  <si>
-    <t>Aficianado's</t>
-  </si>
-  <si>
-    <t>Corey</t>
-  </si>
-  <si>
-    <t>Good Night John Boy</t>
-  </si>
-  <si>
-    <t>Chris</t>
-  </si>
-  <si>
-    <t>Barley Hopster's</t>
-  </si>
-  <si>
-    <t>DJ Rabbit</t>
-  </si>
-  <si>
-    <t>Keith</t>
-  </si>
-  <si>
-    <t>Trivia Goodness</t>
-  </si>
-  <si>
-    <t>Hey Hey Bar &amp; Grill</t>
-  </si>
-  <si>
-    <t>Pint and a Half</t>
-  </si>
-  <si>
-    <t>Zaftig Brewing Company</t>
-  </si>
-  <si>
-    <t>City Tavern Short North</t>
-  </si>
-  <si>
-    <t>Rini</t>
-  </si>
-  <si>
-    <t>Olentangy River Brewing</t>
-  </si>
-  <si>
-    <t>Jarvis</t>
-  </si>
-  <si>
-    <t>Gatsby's</t>
-  </si>
-  <si>
-    <t>CT Audio Productions</t>
-  </si>
-  <si>
-    <t>https://www.triviagoodness.com/play/</t>
-  </si>
-  <si>
-    <t>Keystone Pub &amp; Patio</t>
-  </si>
-  <si>
-    <t>Bada Bean Bada Booze</t>
-  </si>
-  <si>
-    <t>Ethyl &amp; Tank</t>
-  </si>
-  <si>
-    <t>Leiah</t>
-  </si>
-  <si>
-    <t>Park St Tavern</t>
-  </si>
-  <si>
-    <t>Blake</t>
-  </si>
-  <si>
-    <t>Traditions Tavern</t>
-  </si>
-  <si>
-    <t>Question Everything</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Bobcat Sports Bar</t>
-  </si>
-  <si>
-    <t>Baylee</t>
-  </si>
-  <si>
-    <t>Hanks Texas BBQ Clintonville</t>
-  </si>
-  <si>
-    <t>Adam</t>
-  </si>
-  <si>
-    <t>Rule 3</t>
-  </si>
-  <si>
-    <t>The Draft Room</t>
-  </si>
-  <si>
-    <t>Big Head Trivia</t>
-  </si>
-  <si>
-    <t>Budd Dairy</t>
-  </si>
-  <si>
-    <t>Jac &amp; Do's on High</t>
-  </si>
-  <si>
-    <t>Slammers</t>
-  </si>
-  <si>
-    <t>Emaleigh</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/bigheadtrivia/</t>
-  </si>
-  <si>
-    <t>Google Map Links added for all Monday shows on 6/5/24</t>
-  </si>
-  <si>
-    <t>Fenders in Polaris</t>
-  </si>
-  <si>
     <t>Level One Bar + Arcade</t>
   </si>
   <si>
@@ -739,21 +732,27 @@
     <t>The Goat Gahanna</t>
   </si>
   <si>
+    <t>Coaches Bar &amp; Grill</t>
+  </si>
+  <si>
+    <t>Katharine</t>
+  </si>
+  <si>
+    <t>Donericks on High</t>
+  </si>
+  <si>
+    <t>Gemut Biergarten</t>
+  </si>
+  <si>
+    <t>Geeks Who Drink</t>
+  </si>
+  <si>
+    <t>The Goat RiverSouth</t>
+  </si>
+  <si>
     <t>Echo Spirits Distilling Co.</t>
   </si>
   <si>
-    <t>Donericks on High</t>
-  </si>
-  <si>
-    <t>Gemut Biergarten</t>
-  </si>
-  <si>
-    <t>Geeks Who Drink</t>
-  </si>
-  <si>
-    <t>The Goat RiverSouth</t>
-  </si>
-  <si>
     <t>Hop Yard 62 Grove City</t>
   </si>
   <si>
@@ -763,45 +762,48 @@
     <t>North Market Bridge Park</t>
   </si>
   <si>
+    <t>Loose Rail Brewing</t>
+  </si>
+  <si>
+    <t>Google Map Links added for all Weekend shows on 6/13/24</t>
+  </si>
+  <si>
+    <t>Mulligan's Sports Pub</t>
+  </si>
+  <si>
     <t>Local Cantina Clintonville</t>
   </si>
   <si>
-    <t>Loose Rail Brewing</t>
-  </si>
-  <si>
-    <t>Google Map Links added for all Weekend shows on 6/13/24</t>
-  </si>
-  <si>
-    <t>Mulligan's Sports Pub</t>
+    <t>Outerbelt Brewing &amp; Taproom</t>
+  </si>
+  <si>
+    <t>Nasty's</t>
   </si>
   <si>
     <t>Mid City Garage</t>
   </si>
   <si>
-    <t>Outerbelt Brewing &amp; Taproom</t>
-  </si>
-  <si>
-    <t>Nasty's</t>
+    <t>Cassandra</t>
+  </si>
+  <si>
+    <t>Beer Barrel Easton</t>
+  </si>
+  <si>
+    <t>https://wtfmusictrivia.com/play</t>
   </si>
   <si>
     <t>B-Dubs Ohio State</t>
   </si>
   <si>
-    <t>Beer Barrel Easton</t>
-  </si>
-  <si>
-    <t>https://wtfmusictrivia.com/play</t>
+    <t>Donericks Worthington Woods</t>
+  </si>
+  <si>
+    <t>Hale's Ales &amp; Kitchen</t>
   </si>
   <si>
     <t>Blu-Willys</t>
   </si>
   <si>
-    <t>Donericks Worthington Woods</t>
-  </si>
-  <si>
-    <t>Hale's Ales &amp; Kitchen</t>
-  </si>
-  <si>
     <t>Lazy Chameleon</t>
   </si>
   <si>
@@ -817,39 +819,39 @@
     <t>https://www.instagram.com/idrinktrivia/</t>
   </si>
   <si>
+    <t>Land-Grant Brewing</t>
+  </si>
+  <si>
+    <t>BrewDog New Albany</t>
+  </si>
+  <si>
     <t>Wolf's Ridge Brewing Taproom</t>
   </si>
   <si>
-    <t>Land-Grant Brewing</t>
-  </si>
-  <si>
-    <t>BrewDog New Albany</t>
+    <t>Saucy Brew Works</t>
+  </si>
+  <si>
+    <t>Pint and a Half Trivia</t>
+  </si>
+  <si>
+    <t>BrewDog Franklinton</t>
   </si>
   <si>
     <t>The Barn</t>
   </si>
   <si>
-    <t>Saucy Brew Works</t>
-  </si>
-  <si>
-    <t>Pint and a Half Trivia</t>
-  </si>
-  <si>
-    <t>BrewDog Franklinton</t>
+    <t>Slammies on High</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/pintandahalftrivia/</t>
+  </si>
+  <si>
+    <t>BrewDog Canal Winchester</t>
   </si>
   <si>
     <t>Lucky's Grill &amp; Billiards</t>
   </si>
   <si>
-    <t>Slammies on High</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/pintandahalftrivia/</t>
-  </si>
-  <si>
-    <t>BrewDog Canal Winchester</t>
-  </si>
-  <si>
     <t>Eupouria Bar &amp; Patio</t>
   </si>
   <si>
@@ -868,30 +870,30 @@
     <t>Ill Mannered Powell</t>
   </si>
   <si>
+    <t>The Upper Deck</t>
+  </si>
+  <si>
+    <t>Johnny</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/p/Trivia-Night-Ohio-100064713967661/</t>
+  </si>
+  <si>
+    <t>Beer Barrel Dublin</t>
+  </si>
+  <si>
     <t>Eastside Brewing</t>
   </si>
   <si>
-    <t>The Upper Deck</t>
-  </si>
-  <si>
-    <t>Johnny</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/p/Trivia-Night-Ohio-100064713967661/</t>
-  </si>
-  <si>
-    <t>Beer Barrel Dublin</t>
+    <t>Purple Panda Trivia</t>
+  </si>
+  <si>
+    <t>Cuzn'z Bar and Grill</t>
   </si>
   <si>
     <t>Ill Mannered Marysville</t>
   </si>
   <si>
-    <t>Purple Panda Trivia</t>
-  </si>
-  <si>
-    <t>Cuzn'z Bar and Grill</t>
-  </si>
-  <si>
     <t>Somewhere in Particular</t>
   </si>
   <si>
@@ -901,178 +903,178 @@
     <t>Fattey Beer Co</t>
   </si>
   <si>
+    <t>https://columbus-trivia.com/</t>
+  </si>
+  <si>
+    <t>The Grainery</t>
+  </si>
+  <si>
     <t>Oddfellows</t>
   </si>
   <si>
-    <t>https://columbus-trivia.com/</t>
-  </si>
-  <si>
-    <t>The Grainery</t>
+    <t>Powell Bar &amp; Grill</t>
+  </si>
+  <si>
+    <t>Old Dog Alehouse</t>
   </si>
   <si>
     <t>OverTime Sports Pub</t>
   </si>
   <si>
-    <t>Powell Bar &amp; Grill</t>
-  </si>
-  <si>
-    <t>Old Dog Alehouse</t>
+    <t>Combustion Pickerington</t>
+  </si>
+  <si>
+    <t>Crazy Train Trivia</t>
   </si>
   <si>
     <t>TenPin Alley Hilliard</t>
   </si>
   <si>
-    <t>Combustion Pickerington</t>
-  </si>
-  <si>
-    <t>Crazy Train Trivia</t>
+    <t>Bobcat Bar Grandview</t>
+  </si>
+  <si>
+    <t>Self-operated</t>
+  </si>
+  <si>
+    <t>https://instagram.com/mixedologies</t>
+  </si>
+  <si>
+    <t>Rumours</t>
   </si>
   <si>
     <t>The Filling Station Powell</t>
   </si>
   <si>
-    <t>Bobcat Bar Grandview</t>
-  </si>
-  <si>
-    <t>Self-operated</t>
-  </si>
-  <si>
-    <t>https://instagram.com/mixedologies</t>
-  </si>
-  <si>
-    <t>Rumours</t>
+    <t>The Forge Tavern</t>
+  </si>
+  <si>
+    <t>Local Bar</t>
   </si>
   <si>
     <t>Average Joe's Hilliard</t>
   </si>
   <si>
-    <t>The Forge Tavern</t>
-  </si>
-  <si>
-    <t>Local Bar</t>
+    <t>Crooked Can Brewing</t>
   </si>
   <si>
     <t>Beerhead New Albany</t>
   </si>
   <si>
-    <t>Crooked Can Brewing</t>
+    <t>Google Map Links added for all Thursday shows on 6/5/24</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/purple_panda_trivia/</t>
+  </si>
+  <si>
+    <t>Ohio Brewing Company</t>
+  </si>
+  <si>
+    <t>Brook</t>
   </si>
   <si>
     <t>Eldorado's</t>
   </si>
   <si>
-    <t>Google Map Links added for all Thursday shows on 6/5/24</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/purple_panda_trivia/</t>
-  </si>
-  <si>
-    <t>Ohio Brewing Company</t>
-  </si>
-  <si>
-    <t>Brook</t>
-  </si>
-  <si>
     <t>Firehouse Tavern</t>
   </si>
   <si>
+    <t>1801 Tavern Powell</t>
+  </si>
+  <si>
     <t>Jerome Village Bar &amp; Grille</t>
   </si>
   <si>
-    <t>1801 Tavern Powell</t>
+    <t>https://www.facebook.com/CTAudioProductions</t>
+  </si>
+  <si>
+    <t>Pointe Tavern</t>
   </si>
   <si>
     <t>Joe's Pub &amp; Grill Powell</t>
   </si>
   <si>
-    <t>https://www.facebook.com/CTAudioProductions</t>
-  </si>
-  <si>
-    <t>Pointe Tavern</t>
+    <t>Parsons North Brewing</t>
   </si>
   <si>
     <t>New Albany Links Golf Club</t>
   </si>
   <si>
-    <t>Parsons North Brewing</t>
-  </si>
-  <si>
     <t>Question Everything Trivia</t>
   </si>
   <si>
     <t>Signatures Mill Stone Tavern</t>
   </si>
   <si>
+    <t>https://www.facebook.com/qetrivia</t>
+  </si>
+  <si>
+    <t>Classics Pickerington</t>
+  </si>
+  <si>
     <t>Sam</t>
   </si>
   <si>
-    <t>https://www.facebook.com/qetrivia</t>
-  </si>
-  <si>
-    <t>Classics Pickerington</t>
+    <t>Beeline</t>
   </si>
   <si>
     <t>Ashley</t>
   </si>
   <si>
-    <t>Beeline</t>
-  </si>
-  <si>
     <t>Plank's Bier Garten</t>
   </si>
   <si>
+    <t>https://djrabbitevents.com/where-to-play</t>
+  </si>
+  <si>
+    <t>Saturn's Sports Bar</t>
+  </si>
+  <si>
     <t>Town Center Pub</t>
   </si>
   <si>
-    <t>https://djrabbitevents.com/where-to-play</t>
-  </si>
-  <si>
-    <t>Saturn's Sports Bar</t>
+    <t>Shakers Public House</t>
+  </si>
+  <si>
+    <t>Self-operated - Music</t>
   </si>
   <si>
     <t>Tino's Bar &amp; Grille</t>
   </si>
   <si>
-    <t>Shakers Public House</t>
-  </si>
-  <si>
-    <t>Self-operated - Music</t>
+    <t>Turtle Creek Tavern</t>
   </si>
   <si>
     <t>U.A. Pub</t>
   </si>
   <si>
-    <t>Turtle Creek Tavern</t>
+    <t>Union Cafe</t>
+  </si>
+  <si>
+    <t>Blonde Vanity</t>
   </si>
   <si>
     <t>North High Brewing Dublin</t>
   </si>
   <si>
-    <t>Union Cafe</t>
-  </si>
-  <si>
-    <t>Blonde Vanity</t>
-  </si>
-  <si>
     <t>Scoreboard Pub &amp; Grill</t>
   </si>
   <si>
+    <t>Drexel Theater</t>
+  </si>
+  <si>
+    <t>Bexley Library</t>
+  </si>
+  <si>
     <t>Wendell's Pub</t>
   </si>
   <si>
-    <t>Drexel Theater</t>
-  </si>
-  <si>
-    <t>Bexley Library</t>
-  </si>
-  <si>
     <t>Beef 'O' Brady's</t>
   </si>
   <si>
+    <t>Google Map Links added for all Tuesday shows on 11/5/24</t>
+  </si>
+  <si>
     <t>Restoration Brew Worx</t>
-  </si>
-  <si>
-    <t>Google Map Links added for all Tuesday shows on 11/5/24</t>
   </si>
   <si>
     <t>Grandview Cafe</t>
@@ -1100,7 +1102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1212,10 +1214,6 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Archivo Narrow"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
     </font>
     <font>
       <u/>
@@ -1370,7 +1368,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="100">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1549,6 +1547,9 @@
     <xf borderId="0" fillId="18" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="7" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -1556,27 +1557,24 @@
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="15" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="10" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="15" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="17" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
     <xf borderId="0" fillId="10" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -1589,16 +1587,13 @@
     <xf borderId="0" fillId="14" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="14" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="19" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="20" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="20" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
@@ -1631,7 +1626,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="13" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1640,15 +1635,15 @@
     <xf borderId="0" fillId="0" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="9" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
@@ -1664,7 +1659,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -2256,7 +2251,7 @@
         <v>10</v>
       </c>
       <c r="R5" s="8" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="S5" s="9">
         <v>0.3125</v>
@@ -2277,10 +2272,10 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>46</v>
       </c>
       <c r="C6" s="28"/>
       <c r="D6" s="9">
@@ -2288,33 +2283,33 @@
       </c>
       <c r="E6" s="10"/>
       <c r="F6" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I6" s="9">
         <v>0.3333333333333333</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N6" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O6" s="10"/>
       <c r="P6" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q6" s="8" t="s">
         <v>10</v>
@@ -2327,13 +2322,13 @@
       </c>
       <c r="T6" s="10"/>
       <c r="U6" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="V6" s="16" t="s">
         <v>20</v>
       </c>
       <c r="W6" s="29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="X6" s="9">
         <v>0.25</v>
@@ -2351,10 +2346,10 @@
     </row>
     <row r="7">
       <c r="A7" s="31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="9">
@@ -2362,20 +2357,20 @@
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="33" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I7" s="9">
         <v>0.3125</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>10</v>
@@ -2394,7 +2389,7 @@
         <v>10</v>
       </c>
       <c r="R7" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S7" s="9">
         <v>0.3333333333333333</v>
@@ -2407,7 +2402,7 @@
       <c r="Y7" s="10"/>
       <c r="Z7" s="4"/>
       <c r="AA7" s="34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AB7" s="4"/>
       <c r="AC7" s="4"/>
@@ -2417,7 +2412,7 @@
     </row>
     <row r="8">
       <c r="A8" s="31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>18</v>
@@ -2428,46 +2423,46 @@
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="I8" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L8" s="36" t="s">
         <v>10</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N8" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O8" s="10"/>
       <c r="P8" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Q8" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R8" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="S8" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="T8" s="10"/>
       <c r="U8" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="V8" s="1" t="s">
         <v>1</v>
@@ -2489,65 +2484,65 @@
     </row>
     <row r="9">
       <c r="A9" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B9" s="38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C9" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D9" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="E9" s="10"/>
       <c r="F9" s="6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>73</v>
+      <c r="H9" s="12" t="s">
+        <v>70</v>
       </c>
       <c r="I9" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="L9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M9" s="29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="N9" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O9" s="10"/>
       <c r="P9" s="13" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Q9" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R9" s="29" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="S9" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="T9" s="10"/>
       <c r="U9" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="V9" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="W9" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="X9" s="9">
         <v>0.2916666666666667</v>
@@ -2555,7 +2550,7 @@
       <c r="Y9" s="10"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="41" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="AB9" s="4"/>
       <c r="AC9" s="4"/>
@@ -2565,10 +2560,10 @@
     </row>
     <row r="10">
       <c r="A10" s="31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="9">
@@ -2576,7 +2571,7 @@
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>10</v>
@@ -2589,39 +2584,39 @@
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="6" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L10" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M10" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="N10" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O10" s="10"/>
       <c r="P10" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Q10" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R10" s="29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="S10" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="V10" s="43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="W10" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="X10" s="9">
         <v>0.2916666666666667</v>
@@ -2629,7 +2624,7 @@
       <c r="Y10" s="10"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="AB10" s="4"/>
       <c r="AC10" s="4"/>
@@ -2639,20 +2634,20 @@
     </row>
     <row r="11">
       <c r="A11" s="31" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C11" s="40" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D11" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G11" s="29" t="s">
         <v>20</v>
@@ -2665,26 +2660,26 @@
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="L11" s="16" t="s">
         <v>20</v>
       </c>
       <c r="M11" s="37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="N11" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O11" s="10"/>
       <c r="P11" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="Q11" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R11" s="37" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="S11" s="9">
         <v>0.2916666666666667</v>
@@ -2705,46 +2700,46 @@
     </row>
     <row r="12">
       <c r="A12" s="31" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B12" s="45" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D12" s="9">
         <v>0.3333333333333333</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="33" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G12" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H12" s="46" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="I12" s="9">
         <v>0.3333333333333333</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L12" s="16" t="s">
         <v>20</v>
       </c>
       <c r="M12" s="37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="N12" s="9">
         <v>0.3333333333333333</v>
       </c>
       <c r="O12" s="10"/>
       <c r="P12" s="13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="Q12" s="29" t="s">
         <v>20</v>
@@ -2757,10 +2752,10 @@
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="V12" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="W12" s="47"/>
       <c r="X12" s="9">
@@ -2769,7 +2764,7 @@
       <c r="Y12" s="10"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="48" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="AB12" s="4"/>
       <c r="AC12" s="4"/>
@@ -2784,7 +2779,7 @@
       <c r="D13" s="25"/>
       <c r="E13" s="10"/>
       <c r="F13" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G13" s="29" t="s">
         <v>20</v>
@@ -2797,26 +2792,26 @@
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="31" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L13" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M13" s="50" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N13" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O13" s="10"/>
       <c r="P13" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="Q13" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R13" s="29" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="S13" s="9">
         <v>0.2916666666666667</v>
@@ -2829,7 +2824,7 @@
       <c r="Y13" s="10"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="23" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="AB13" s="4"/>
       <c r="AC13" s="4"/>
@@ -2839,27 +2834,27 @@
     </row>
     <row r="14">
       <c r="A14" s="49" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B14" s="25"/>
       <c r="C14" s="25"/>
       <c r="D14" s="25"/>
       <c r="E14" s="10"/>
       <c r="F14" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="29" t="s">
-        <v>48</v>
+        <v>112</v>
       </c>
       <c r="I14" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="L14" s="29" t="s">
         <v>20</v>
@@ -2872,13 +2867,13 @@
       </c>
       <c r="O14" s="10"/>
       <c r="P14" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q14" s="29" t="s">
         <v>20</v>
       </c>
       <c r="R14" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="S14" s="9">
         <v>0.3333333333333333</v>
@@ -2904,36 +2899,36 @@
       <c r="D15" s="25"/>
       <c r="E15" s="10"/>
       <c r="F15" s="13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G15" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H15" s="29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="I15" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="L15" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M15" s="29" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="N15" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="Q15" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R15" s="51"/>
       <c r="S15" s="9">
@@ -2941,7 +2936,7 @@
       </c>
       <c r="T15" s="10"/>
       <c r="U15" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>1</v>
@@ -2955,7 +2950,7 @@
       <c r="Y15" s="10"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="52" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AB15" s="4"/>
       <c r="AC15" s="4"/>
@@ -2965,43 +2960,43 @@
     </row>
     <row r="16">
       <c r="A16" s="53" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="10"/>
       <c r="F16" s="13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="29" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I16" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M16" s="37" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="N16" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O16" s="10"/>
       <c r="P16" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q16" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R16" s="51"/>
       <c r="S16" s="9">
@@ -3009,13 +3004,13 @@
       </c>
       <c r="T16" s="10"/>
       <c r="U16" s="13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="V16" s="29" t="s">
         <v>20</v>
       </c>
       <c r="W16" s="37" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="X16" s="9">
         <v>0.25</v>
@@ -3023,7 +3018,7 @@
       <c r="Y16" s="10"/>
       <c r="Z16" s="4"/>
       <c r="AA16" s="23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
@@ -3033,43 +3028,43 @@
     </row>
     <row r="17">
       <c r="A17" s="49" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17" s="25"/>
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="10"/>
       <c r="F17" s="13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G17" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H17" s="29" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I17" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L17" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M17" s="29" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N17" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O17" s="10"/>
       <c r="P17" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q17" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R17" s="54"/>
       <c r="S17" s="9">
@@ -3077,7 +3072,7 @@
       </c>
       <c r="T17" s="10"/>
       <c r="U17" s="13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="V17" s="29" t="s">
         <v>20</v>
@@ -3099,43 +3094,43 @@
     </row>
     <row r="18">
       <c r="A18" s="49" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="25"/>
       <c r="E18" s="10"/>
       <c r="F18" s="13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G18" s="29" t="s">
         <v>20</v>
       </c>
       <c r="H18" s="29" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="I18" s="9">
         <v>0.2708333333333333</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L18" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M18" s="29" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="N18" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O18" s="10"/>
       <c r="P18" s="13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="Q18" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="R18" s="51"/>
       <c r="S18" s="9">
@@ -3143,10 +3138,10 @@
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="31" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="V18" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="W18" s="55"/>
       <c r="X18" s="9">
@@ -3155,7 +3150,7 @@
       <c r="Y18" s="10"/>
       <c r="Z18" s="4"/>
       <c r="AA18" s="56" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AB18" s="4"/>
       <c r="AC18" s="4"/>
@@ -3165,27 +3160,27 @@
     </row>
     <row r="19">
       <c r="A19" s="49" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
       <c r="E19" s="57"/>
       <c r="F19" s="33" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G19" s="46" t="s">
         <v>20</v>
       </c>
       <c r="H19" s="46" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I19" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="L19" s="29" t="s">
         <v>20</v>
@@ -3198,10 +3193,10 @@
       </c>
       <c r="O19" s="57"/>
       <c r="P19" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q19" s="58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="R19" s="58"/>
       <c r="S19" s="9">
@@ -3209,10 +3204,10 @@
       </c>
       <c r="T19" s="57"/>
       <c r="U19" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="V19" s="59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="W19" s="59"/>
       <c r="X19" s="9">
@@ -3221,7 +3216,7 @@
       <c r="Y19" s="57"/>
       <c r="Z19" s="4"/>
       <c r="AA19" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AB19" s="22"/>
       <c r="AC19" s="22"/>
@@ -3236,10 +3231,10 @@
       <c r="D20" s="25"/>
       <c r="E20" s="57"/>
       <c r="F20" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="9">
@@ -3247,23 +3242,23 @@
       </c>
       <c r="J20" s="10"/>
       <c r="K20" s="13" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L20" s="29" t="s">
         <v>20</v>
       </c>
       <c r="M20" s="29" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="N20" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O20" s="57"/>
       <c r="P20" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q20" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R20" s="47"/>
       <c r="S20" s="9">
@@ -3271,13 +3266,13 @@
       </c>
       <c r="T20" s="57"/>
       <c r="U20" s="13" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="V20" s="13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="W20" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="X20" s="9">
         <v>0.2708333333333333</v>
@@ -3298,32 +3293,34 @@
       <c r="D21" s="25"/>
       <c r="E21" s="57"/>
       <c r="F21" s="13" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H21" s="28"/>
       <c r="I21" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J21" s="10"/>
-      <c r="K21" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="L21" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="M21" s="28"/>
+      <c r="K21" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="L21" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="M21" s="60" t="s">
+        <v>157</v>
+      </c>
       <c r="N21" s="9">
         <v>0.2708333333333333</v>
       </c>
       <c r="O21" s="57"/>
       <c r="P21" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="Q21" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R21" s="47"/>
       <c r="S21" s="9">
@@ -3331,10 +3328,10 @@
       </c>
       <c r="T21" s="57"/>
       <c r="U21" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="V21" s="22" t="s">
         <v>160</v>
-      </c>
-      <c r="V21" s="22" t="s">
-        <v>161</v>
       </c>
       <c r="W21" s="4"/>
       <c r="X21" s="9">
@@ -3342,8 +3339,8 @@
       </c>
       <c r="Y21" s="57"/>
       <c r="Z21" s="4"/>
-      <c r="AA21" s="60" t="s">
-        <v>55</v>
+      <c r="AA21" s="61" t="s">
+        <v>53</v>
       </c>
       <c r="AB21" s="4"/>
       <c r="AC21" s="4"/>
@@ -3352,38 +3349,38 @@
       <c r="AF21" s="4"/>
     </row>
     <row r="22">
-      <c r="A22" s="61"/>
-      <c r="B22" s="61"/>
-      <c r="C22" s="61"/>
-      <c r="D22" s="61"/>
+      <c r="A22" s="62"/>
+      <c r="B22" s="62"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="57"/>
       <c r="F22" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H22" s="28"/>
       <c r="I22" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J22" s="57"/>
-      <c r="K22" s="6" t="s">
-        <v>160</v>
+      <c r="K22" s="13" t="s">
+        <v>162</v>
       </c>
       <c r="L22" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M22" s="28"/>
       <c r="N22" s="9">
-        <v>0.3125</v>
+        <v>0.2708333333333333</v>
       </c>
       <c r="O22" s="57"/>
       <c r="P22" s="13" t="s">
         <v>163</v>
       </c>
       <c r="Q22" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R22" s="47"/>
       <c r="S22" s="9">
@@ -3415,29 +3412,29 @@
         <v>165</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23" s="28"/>
       <c r="I23" s="9">
         <v>0.25</v>
       </c>
       <c r="J23" s="57"/>
-      <c r="K23" s="13" t="s">
-        <v>166</v>
+      <c r="K23" s="6" t="s">
+        <v>159</v>
       </c>
       <c r="L23" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M23" s="28"/>
       <c r="N23" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="O23" s="57"/>
       <c r="P23" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="Q23" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R23" s="47"/>
       <c r="S23" s="9">
@@ -3445,7 +3442,7 @@
       </c>
       <c r="T23" s="57"/>
       <c r="U23" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
@@ -3460,27 +3457,27 @@
       <c r="AF23" s="4"/>
     </row>
     <row r="24">
-      <c r="A24" s="61"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
+      <c r="A24" s="62"/>
+      <c r="B24" s="62"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
       <c r="E24" s="57"/>
       <c r="F24" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H24" s="51"/>
       <c r="I24" s="9">
         <v>0.3125</v>
       </c>
       <c r="J24" s="57"/>
-      <c r="K24" s="6" t="s">
-        <v>170</v>
+      <c r="K24" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="L24" s="28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M24" s="28"/>
       <c r="N24" s="9">
@@ -3488,10 +3485,10 @@
       </c>
       <c r="O24" s="57"/>
       <c r="P24" s="13" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q24" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R24" s="47"/>
       <c r="S24" s="9">
@@ -3504,7 +3501,7 @@
       <c r="X24" s="25"/>
       <c r="Y24" s="57"/>
       <c r="Z24" s="4"/>
-      <c r="AA24" s="62" t="s">
+      <c r="AA24" s="63" t="s">
         <v>18</v>
       </c>
       <c r="AB24" s="4"/>
@@ -3514,40 +3511,42 @@
       <c r="AF24" s="4"/>
     </row>
     <row r="25">
-      <c r="A25" s="61"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
+      <c r="A25" s="62"/>
+      <c r="B25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="57"/>
       <c r="F25" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G25" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H25" s="51"/>
       <c r="I25" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J25" s="57"/>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="M25" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="L25" s="63" t="s">
-        <v>81</v>
-      </c>
-      <c r="M25" s="64"/>
       <c r="N25" s="9">
-        <v>0.3125</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O25" s="57"/>
       <c r="P25" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="Q25" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="R25" s="65"/>
+      <c r="Q25" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="R25" s="64"/>
       <c r="S25" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -3574,32 +3573,32 @@
       <c r="D26" s="25"/>
       <c r="E26" s="57"/>
       <c r="F26" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G26" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H26" s="51"/>
       <c r="I26" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J26" s="57"/>
-      <c r="K26" s="13" t="s">
+      <c r="K26" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="L26" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="M26" s="54"/>
+      <c r="L26" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="M26" s="65"/>
       <c r="N26" s="9">
-        <v>0.2708333333333333</v>
+        <v>0.3125</v>
       </c>
       <c r="O26" s="57"/>
       <c r="P26" s="13" t="s">
         <v>177</v>
       </c>
       <c r="Q26" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R26" s="55"/>
       <c r="S26" s="9">
@@ -3629,31 +3628,31 @@
         <v>178</v>
       </c>
       <c r="G27" s="66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H27" s="66" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I27" s="9">
         <v>0.3125</v>
       </c>
       <c r="J27" s="57"/>
-      <c r="K27" s="6" t="s">
-        <v>169</v>
+      <c r="K27" s="13" t="s">
+        <v>179</v>
       </c>
       <c r="L27" s="51" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="M27" s="54"/>
       <c r="N27" s="9">
-        <v>0.3125</v>
+        <v>0.2708333333333333</v>
       </c>
       <c r="O27" s="57"/>
       <c r="P27" s="13" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="Q27" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R27" s="55"/>
       <c r="S27" s="9">
@@ -3667,7 +3666,7 @@
       <c r="Y27" s="57"/>
       <c r="Z27" s="4"/>
       <c r="AA27" s="67" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="AB27" s="4"/>
       <c r="AC27" s="4"/>
@@ -3685,7 +3684,7 @@
         <v>15</v>
       </c>
       <c r="G28" s="66" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H28" s="66"/>
       <c r="I28" s="9">
@@ -3693,24 +3692,24 @@
       </c>
       <c r="J28" s="57"/>
       <c r="K28" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="L28" s="68" t="s">
-        <v>81</v>
+        <v>168</v>
+      </c>
+      <c r="L28" s="51" t="s">
+        <v>78</v>
       </c>
       <c r="M28" s="54"/>
       <c r="N28" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="O28" s="57"/>
       <c r="P28" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="Q28" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="R28" s="55" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="S28" s="9">
         <v>0.2916666666666667</v>
@@ -3722,8 +3721,8 @@
       <c r="X28" s="25"/>
       <c r="Y28" s="57"/>
       <c r="Z28" s="4"/>
-      <c r="AA28" s="69" t="s">
-        <v>183</v>
+      <c r="AA28" s="68" t="s">
+        <v>184</v>
       </c>
       <c r="AB28" s="4"/>
       <c r="AC28" s="4"/>
@@ -3738,10 +3737,10 @@
       <c r="D29" s="25"/>
       <c r="E29" s="57"/>
       <c r="F29" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G29" s="58" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H29" s="58"/>
       <c r="I29" s="9">
@@ -3749,10 +3748,10 @@
       </c>
       <c r="J29" s="57"/>
       <c r="K29" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="L29" s="68" t="s">
-        <v>81</v>
+        <v>133</v>
+      </c>
+      <c r="L29" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="M29" s="54"/>
       <c r="N29" s="9">
@@ -3793,7 +3792,7 @@
         <v>186</v>
       </c>
       <c r="G30" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H30" s="47"/>
       <c r="I30" s="9">
@@ -3803,12 +3802,12 @@
       <c r="K30" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="L30" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="M30" s="58"/>
+      <c r="L30" s="69" t="s">
+        <v>78</v>
+      </c>
+      <c r="M30" s="54"/>
       <c r="N30" s="9">
-        <v>0.3125</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O30" s="57"/>
       <c r="P30" s="13" t="s">
@@ -3847,7 +3846,7 @@
         <v>190</v>
       </c>
       <c r="G31" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H31" s="47"/>
       <c r="I31" s="9">
@@ -3857,10 +3856,10 @@
       <c r="K31" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="L31" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="M31" s="71"/>
+      <c r="L31" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="M31" s="58"/>
       <c r="N31" s="9">
         <v>0.3125</v>
       </c>
@@ -3882,7 +3881,7 @@
       <c r="X31" s="25"/>
       <c r="Y31" s="57"/>
       <c r="Z31" s="4"/>
-      <c r="AA31" s="69" t="s">
+      <c r="AA31" s="68" t="s">
         <v>193</v>
       </c>
       <c r="AB31" s="4"/>
@@ -3901,7 +3900,7 @@
         <v>194</v>
       </c>
       <c r="G32" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H32" s="47"/>
       <c r="I32" s="9">
@@ -3909,24 +3908,24 @@
       </c>
       <c r="J32" s="57"/>
       <c r="K32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L32" s="58" t="s">
-        <v>148</v>
-      </c>
-      <c r="M32" s="58"/>
+        <v>195</v>
+      </c>
+      <c r="L32" s="71" t="s">
+        <v>146</v>
+      </c>
+      <c r="M32" s="71"/>
       <c r="N32" s="9">
         <v>0.3125</v>
       </c>
       <c r="O32" s="57"/>
       <c r="P32" s="13" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="Q32" s="72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="R32" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="S32" s="9">
         <v>0.3125</v>
@@ -3952,35 +3951,35 @@
       <c r="D33" s="25"/>
       <c r="E33" s="57"/>
       <c r="F33" s="33" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G33" s="73" t="s">
-        <v>107</v>
-      </c>
-      <c r="H33" s="74"/>
+        <v>104</v>
+      </c>
+      <c r="H33" s="73"/>
       <c r="I33" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J33" s="57"/>
-      <c r="K33" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="L33" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="M33" s="47"/>
+      <c r="K33" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="58" t="s">
+        <v>146</v>
+      </c>
+      <c r="M33" s="58"/>
       <c r="N33" s="9">
-        <v>0.2708333333333333</v>
+        <v>0.3125</v>
       </c>
       <c r="O33" s="57"/>
       <c r="P33" s="13" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="Q33" s="72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="R33" s="72" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="S33" s="9">
         <v>0.3125</v>
@@ -3992,8 +3991,8 @@
       <c r="X33" s="25"/>
       <c r="Y33" s="57"/>
       <c r="Z33" s="4"/>
-      <c r="AA33" s="75" t="s">
-        <v>199</v>
+      <c r="AA33" s="74" t="s">
+        <v>200</v>
       </c>
       <c r="AB33" s="4"/>
       <c r="AC33" s="4"/>
@@ -4008,10 +4007,10 @@
       <c r="D34" s="25"/>
       <c r="E34" s="57"/>
       <c r="F34" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G34" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H34" s="47"/>
       <c r="I34" s="9">
@@ -4019,23 +4018,23 @@
       </c>
       <c r="J34" s="57"/>
       <c r="K34" s="13" t="s">
-        <v>201</v>
+        <v>103</v>
       </c>
       <c r="L34" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M34" s="47"/>
       <c r="N34" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.2708333333333333</v>
       </c>
       <c r="O34" s="57"/>
       <c r="P34" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="Q34" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="R34" s="76" t="s">
+      <c r="Q34" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="R34" s="75" t="s">
         <v>203</v>
       </c>
       <c r="S34" s="9">
@@ -4048,7 +4047,7 @@
       <c r="X34" s="25"/>
       <c r="Y34" s="57"/>
       <c r="Z34" s="4"/>
-      <c r="AA34" s="77" t="s">
+      <c r="AA34" s="76" t="s">
         <v>204</v>
       </c>
       <c r="AB34" s="4"/>
@@ -4066,10 +4065,10 @@
       <c r="F35" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="G35" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="H35" s="65"/>
+      <c r="G35" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="H35" s="64"/>
       <c r="I35" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>206</v>
       </c>
       <c r="L35" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M35" s="47"/>
       <c r="N35" s="9">
@@ -4086,12 +4085,12 @@
       </c>
       <c r="O35" s="57"/>
       <c r="P35" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q35" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q35" s="77" t="s">
         <v>207</v>
       </c>
-      <c r="R35" s="78"/>
+      <c r="R35" s="77"/>
       <c r="S35" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4119,7 +4118,7 @@
         <v>208</v>
       </c>
       <c r="G36" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H36" s="55"/>
       <c r="I36" s="9">
@@ -4127,10 +4126,10 @@
       </c>
       <c r="J36" s="57"/>
       <c r="K36" s="13" t="s">
-        <v>167</v>
+        <v>209</v>
       </c>
       <c r="L36" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M36" s="47"/>
       <c r="N36" s="9">
@@ -4138,13 +4137,13 @@
       </c>
       <c r="O36" s="57"/>
       <c r="P36" s="13" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="Q36" s="43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="R36" s="44" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="S36" s="9">
         <v>0.2916666666666667</v>
@@ -4156,8 +4155,8 @@
       <c r="X36" s="25"/>
       <c r="Y36" s="57"/>
       <c r="Z36" s="4"/>
-      <c r="AA36" s="79" t="s">
-        <v>210</v>
+      <c r="AA36" s="78" t="s">
+        <v>211</v>
       </c>
       <c r="AB36" s="4"/>
       <c r="AC36" s="4"/>
@@ -4172,10 +4171,10 @@
       <c r="D37" s="25"/>
       <c r="E37" s="57"/>
       <c r="F37" s="13" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G37" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H37" s="55"/>
       <c r="I37" s="9">
@@ -4183,10 +4182,10 @@
       </c>
       <c r="J37" s="57"/>
       <c r="K37" s="13" t="s">
-        <v>212</v>
+        <v>166</v>
       </c>
       <c r="L37" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M37" s="47"/>
       <c r="N37" s="9">
@@ -4194,10 +4193,10 @@
       </c>
       <c r="O37" s="57"/>
       <c r="P37" s="31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Q37" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="R37" s="40"/>
       <c r="S37" s="9">
@@ -4229,7 +4228,7 @@
         <v>214</v>
       </c>
       <c r="G38" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H38" s="55"/>
       <c r="I38" s="9">
@@ -4240,7 +4239,7 @@
         <v>215</v>
       </c>
       <c r="L38" s="47" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M38" s="47"/>
       <c r="N38" s="9">
@@ -4251,7 +4250,7 @@
         <v>216</v>
       </c>
       <c r="Q38" s="39" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="R38" s="40"/>
       <c r="S38" s="9">
@@ -4281,7 +4280,7 @@
         <v>217</v>
       </c>
       <c r="G39" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H39" s="55"/>
       <c r="I39" s="9">
@@ -4291,21 +4290,21 @@
       <c r="K39" s="13" t="s">
         <v>218</v>
       </c>
-      <c r="L39" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="M39" s="65"/>
+      <c r="L39" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="M39" s="47"/>
       <c r="N39" s="9">
-        <v>0.2708333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O39" s="57"/>
       <c r="P39" s="6" t="s">
         <v>219</v>
       </c>
-      <c r="Q39" s="80" t="s">
+      <c r="Q39" s="79" t="s">
         <v>220</v>
       </c>
-      <c r="R39" s="80"/>
+      <c r="R39" s="79"/>
       <c r="S39" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4316,8 +4315,8 @@
       <c r="X39" s="25"/>
       <c r="Y39" s="57"/>
       <c r="Z39" s="4"/>
-      <c r="AA39" s="81" t="s">
-        <v>150</v>
+      <c r="AA39" s="80" t="s">
+        <v>148</v>
       </c>
       <c r="AB39" s="4"/>
       <c r="AC39" s="4"/>
@@ -4332,10 +4331,10 @@
       <c r="D40" s="25"/>
       <c r="E40" s="57"/>
       <c r="F40" s="13" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G40" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H40" s="55"/>
       <c r="I40" s="9">
@@ -4345,12 +4344,12 @@
       <c r="K40" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="L40" s="65" t="s">
-        <v>122</v>
-      </c>
-      <c r="M40" s="65"/>
+      <c r="L40" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="M40" s="64"/>
       <c r="N40" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.2708333333333333</v>
       </c>
       <c r="O40" s="57"/>
       <c r="P40" s="33" t="s">
@@ -4399,10 +4398,10 @@
       <c r="K41" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="L41" s="55" t="s">
-        <v>55</v>
-      </c>
-      <c r="M41" s="55"/>
+      <c r="L41" s="64" t="s">
+        <v>120</v>
+      </c>
+      <c r="M41" s="64"/>
       <c r="N41" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4452,7 +4451,7 @@
         <v>229</v>
       </c>
       <c r="L42" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M42" s="55"/>
       <c r="N42" s="9">
@@ -4470,7 +4469,7 @@
       <c r="X42" s="25"/>
       <c r="Y42" s="57"/>
       <c r="Z42" s="4"/>
-      <c r="AA42" s="82" t="s">
+      <c r="AA42" s="81" t="s">
         <v>207</v>
       </c>
       <c r="AB42" s="4"/>
@@ -4489,10 +4488,10 @@
         <v>230</v>
       </c>
       <c r="G43" s="72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I43" s="9">
         <v>0.2708333333333333</v>
@@ -4502,11 +4501,11 @@
         <v>231</v>
       </c>
       <c r="L43" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M43" s="55"/>
       <c r="N43" s="9">
-        <v>0.3125</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O43" s="57"/>
       <c r="P43" s="22" t="s">
@@ -4522,7 +4521,7 @@
       <c r="X43" s="25"/>
       <c r="Y43" s="57"/>
       <c r="Z43" s="4"/>
-      <c r="AA43" s="69" t="s">
+      <c r="AA43" s="68" t="s">
         <v>233</v>
       </c>
       <c r="AB43" s="4"/>
@@ -4541,7 +4540,7 @@
         <v>234</v>
       </c>
       <c r="G44" s="38" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="H44" s="38" t="s">
         <v>235</v>
@@ -4554,11 +4553,11 @@
         <v>236</v>
       </c>
       <c r="L44" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M44" s="55"/>
       <c r="N44" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="O44" s="57"/>
       <c r="P44" s="4"/>
@@ -4586,12 +4585,12 @@
       <c r="D45" s="25"/>
       <c r="E45" s="57"/>
       <c r="F45" s="31" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="G45" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="H45" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="H45" s="75" t="s">
         <v>203</v>
       </c>
       <c r="I45" s="9">
@@ -4602,11 +4601,11 @@
         <v>237</v>
       </c>
       <c r="L45" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M45" s="55"/>
       <c r="N45" s="9">
-        <v>0.2708333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O45" s="57"/>
       <c r="P45" s="4"/>
@@ -4620,8 +4619,8 @@
       <c r="X45" s="25"/>
       <c r="Y45" s="57"/>
       <c r="Z45" s="4"/>
-      <c r="AA45" s="83" t="s">
-        <v>90</v>
+      <c r="AA45" s="82" t="s">
+        <v>87</v>
       </c>
       <c r="AB45" s="4"/>
       <c r="AC45" s="4"/>
@@ -4638,10 +4637,10 @@
       <c r="F46" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="G46" s="84" t="s">
-        <v>199</v>
-      </c>
-      <c r="H46" s="84"/>
+      <c r="G46" s="83" t="s">
+        <v>200</v>
+      </c>
+      <c r="H46" s="83"/>
       <c r="I46" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>239</v>
       </c>
       <c r="L46" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M46" s="55"/>
       <c r="N46" s="9">
@@ -4668,7 +4667,7 @@
       <c r="X46" s="25"/>
       <c r="Y46" s="57"/>
       <c r="Z46" s="4"/>
-      <c r="AA46" s="69" t="s">
+      <c r="AA46" s="68" t="s">
         <v>240</v>
       </c>
       <c r="AB46" s="4"/>
@@ -4686,10 +4685,10 @@
       <c r="F47" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="G47" s="84" t="s">
-        <v>199</v>
-      </c>
-      <c r="H47" s="84"/>
+      <c r="G47" s="83" t="s">
+        <v>200</v>
+      </c>
+      <c r="H47" s="83"/>
       <c r="I47" s="9">
         <v>0.3333333333333333</v>
       </c>
@@ -4698,7 +4697,7 @@
         <v>242</v>
       </c>
       <c r="L47" s="55" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="M47" s="55"/>
       <c r="N47" s="9">
@@ -4716,7 +4715,7 @@
       <c r="X47" s="25"/>
       <c r="Y47" s="57"/>
       <c r="Z47" s="4"/>
-      <c r="AA47" s="80"/>
+      <c r="AA47" s="79"/>
       <c r="AB47" s="4"/>
       <c r="AC47" s="4"/>
       <c r="AD47" s="25"/>
@@ -4732,23 +4731,23 @@
       <c r="F48" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="G48" s="85" t="s">
-        <v>150</v>
-      </c>
-      <c r="H48" s="85"/>
+      <c r="G48" s="84" t="s">
+        <v>148</v>
+      </c>
+      <c r="H48" s="84"/>
       <c r="I48" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="J48" s="57"/>
       <c r="K48" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="L48" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="M48" s="14"/>
+        <v>244</v>
+      </c>
+      <c r="L48" s="55" t="s">
+        <v>53</v>
+      </c>
+      <c r="M48" s="55"/>
       <c r="N48" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.2708333333333333</v>
       </c>
       <c r="O48" s="57"/>
       <c r="P48" s="4"/>
@@ -4762,8 +4761,8 @@
       <c r="X48" s="25"/>
       <c r="Y48" s="57"/>
       <c r="Z48" s="4"/>
-      <c r="AA48" s="86" t="s">
-        <v>244</v>
+      <c r="AA48" s="85" t="s">
+        <v>245</v>
       </c>
       <c r="AB48" s="4"/>
       <c r="AC48" s="4"/>
@@ -4778,27 +4777,25 @@
       <c r="D49" s="25"/>
       <c r="E49" s="57"/>
       <c r="F49" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G49" s="43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H49" s="44" t="s">
-        <v>77</v>
-      </c>
-      <c r="I49" s="87">
+        <v>74</v>
+      </c>
+      <c r="I49" s="86">
         <v>0.2916666666666667</v>
       </c>
       <c r="J49" s="57"/>
       <c r="K49" s="13" t="s">
-        <v>234</v>
+        <v>126</v>
       </c>
       <c r="L49" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M49" s="14" t="s">
-        <v>246</v>
-      </c>
+      <c r="M49" s="14"/>
       <c r="N49" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -4814,7 +4811,7 @@
       <c r="X49" s="25"/>
       <c r="Y49" s="57"/>
       <c r="Z49" s="4"/>
-      <c r="AA49" s="88" t="s">
+      <c r="AA49" s="87" t="s">
         <v>247</v>
       </c>
       <c r="AB49" s="4"/>
@@ -4832,23 +4829,23 @@
       <c r="F50" s="33" t="s">
         <v>248</v>
       </c>
-      <c r="G50" s="89" t="s">
-        <v>99</v>
-      </c>
-      <c r="H50" s="90" t="s">
-        <v>100</v>
+      <c r="G50" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="H50" s="89" t="s">
+        <v>97</v>
       </c>
       <c r="I50" s="9">
         <v>0.3125</v>
       </c>
       <c r="J50" s="57"/>
-      <c r="K50" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L50" s="91" t="s">
+      <c r="K50" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="L50" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="M50" s="92" t="s">
+      <c r="M50" s="14" t="s">
         <v>249</v>
       </c>
       <c r="N50" s="9">
@@ -4882,7 +4879,7 @@
       <c r="F51" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="G51" s="93" t="s">
+      <c r="G51" s="90" t="s">
         <v>223</v>
       </c>
       <c r="H51" s="4"/>
@@ -4890,17 +4887,17 @@
         <v>0.25</v>
       </c>
       <c r="J51" s="57"/>
-      <c r="K51" s="13" t="s">
+      <c r="K51" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L51" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="M51" s="92" t="s">
         <v>251</v>
       </c>
-      <c r="L51" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="M51" s="38" t="s">
-        <v>71</v>
-      </c>
       <c r="N51" s="9">
-        <v>0.3125</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O51" s="57"/>
       <c r="P51" s="4"/>
@@ -4914,8 +4911,8 @@
       <c r="X51" s="25"/>
       <c r="Y51" s="57"/>
       <c r="Z51" s="4"/>
-      <c r="AA51" s="94" t="s">
-        <v>79</v>
+      <c r="AA51" s="93" t="s">
+        <v>76</v>
       </c>
       <c r="AB51" s="4"/>
       <c r="AC51" s="4"/>
@@ -4932,7 +4929,7 @@
       <c r="F52" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="G52" s="93" t="s">
+      <c r="G52" s="90" t="s">
         <v>223</v>
       </c>
       <c r="H52" s="4"/>
@@ -4943,14 +4940,14 @@
       <c r="K52" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="L52" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="M52" s="76" t="s">
-        <v>203</v>
+      <c r="L52" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="M52" s="38" t="s">
+        <v>68</v>
       </c>
       <c r="N52" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="O52" s="57"/>
       <c r="P52" s="4"/>
@@ -4964,7 +4961,7 @@
       <c r="X52" s="25"/>
       <c r="Y52" s="57"/>
       <c r="Z52" s="4"/>
-      <c r="AA52" s="88" t="s">
+      <c r="AA52" s="87" t="s">
         <v>253</v>
       </c>
       <c r="AB52" s="4"/>
@@ -4982,7 +4979,7 @@
       <c r="F53" s="6" t="s">
         <v>254</v>
       </c>
-      <c r="G53" s="93" t="s">
+      <c r="G53" s="90" t="s">
         <v>223</v>
       </c>
       <c r="H53" s="4"/>
@@ -4993,12 +4990,14 @@
       <c r="K53" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="L53" s="95" t="s">
-        <v>199</v>
-      </c>
-      <c r="M53" s="95"/>
+      <c r="L53" s="75" t="s">
+        <v>80</v>
+      </c>
+      <c r="M53" s="75" t="s">
+        <v>203</v>
+      </c>
       <c r="N53" s="9">
-        <v>0.3333333333333333</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="O53" s="57"/>
       <c r="P53" s="4"/>
@@ -5028,7 +5027,7 @@
       <c r="F54" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="G54" s="93" t="s">
+      <c r="G54" s="90" t="s">
         <v>257</v>
       </c>
       <c r="H54" s="4"/>
@@ -5039,10 +5038,10 @@
       <c r="K54" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="L54" s="95" t="s">
-        <v>199</v>
-      </c>
-      <c r="M54" s="95"/>
+      <c r="L54" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="M54" s="94"/>
       <c r="N54" s="9">
         <v>0.3333333333333333</v>
       </c>
@@ -5074,7 +5073,7 @@
       <c r="F55" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="G55" s="93" t="s">
+      <c r="G55" s="90" t="s">
         <v>223</v>
       </c>
       <c r="H55" s="4"/>
@@ -5085,12 +5084,12 @@
       <c r="K55" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="L55" s="85" t="s">
-        <v>150</v>
-      </c>
-      <c r="M55" s="85"/>
+      <c r="L55" s="94" t="s">
+        <v>200</v>
+      </c>
+      <c r="M55" s="94"/>
       <c r="N55" s="9">
-        <v>0.25</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="O55" s="57"/>
       <c r="P55" s="4"/>
@@ -5116,11 +5115,11 @@
       <c r="B56" s="25"/>
       <c r="C56" s="25"/>
       <c r="D56" s="25"/>
-      <c r="E56" s="96"/>
+      <c r="E56" s="95"/>
       <c r="F56" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="G56" s="93" t="s">
+      <c r="G56" s="90" t="s">
         <v>223</v>
       </c>
       <c r="H56" s="22" t="s">
@@ -5129,18 +5128,16 @@
       <c r="I56" s="9">
         <v>0.2916666666666667</v>
       </c>
-      <c r="J56" s="96"/>
-      <c r="K56" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="L56" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="M56" s="44" t="s">
-        <v>77</v>
-      </c>
+      <c r="J56" s="95"/>
+      <c r="K56" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="L56" s="84" t="s">
+        <v>148</v>
+      </c>
+      <c r="M56" s="84"/>
       <c r="N56" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.25</v>
       </c>
       <c r="O56" s="57"/>
       <c r="P56" s="4"/>
@@ -5166,26 +5163,26 @@
       <c r="B57" s="25"/>
       <c r="C57" s="25"/>
       <c r="D57" s="25"/>
-      <c r="E57" s="96"/>
+      <c r="E57" s="95"/>
       <c r="F57" s="33" t="s">
-        <v>263</v>
-      </c>
-      <c r="G57" s="90" t="s">
+        <v>264</v>
+      </c>
+      <c r="G57" s="89" t="s">
         <v>223</v>
       </c>
-      <c r="H57" s="90"/>
+      <c r="H57" s="89"/>
       <c r="I57" s="9">
         <v>0.3333333333333333</v>
       </c>
-      <c r="J57" s="97"/>
-      <c r="K57" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="L57" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="M57" s="40" t="s">
-        <v>249</v>
+      <c r="J57" s="96"/>
+      <c r="K57" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="L57" s="43" t="s">
+        <v>87</v>
+      </c>
+      <c r="M57" s="44" t="s">
+        <v>74</v>
       </c>
       <c r="N57" s="9">
         <v>0.2916666666666667</v>
@@ -5214,7 +5211,7 @@
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
       <c r="D58" s="25"/>
-      <c r="E58" s="96"/>
+      <c r="E58" s="95"/>
       <c r="F58" s="13" t="s">
         <v>265</v>
       </c>
@@ -5225,15 +5222,17 @@
       <c r="I58" s="9">
         <v>0.2916666666666667</v>
       </c>
-      <c r="J58" s="97"/>
-      <c r="K58" s="6" t="s">
+      <c r="J58" s="96"/>
+      <c r="K58" s="24" t="s">
         <v>267</v>
       </c>
-      <c r="L58" s="93" t="s">
-        <v>161</v>
-      </c>
-      <c r="M58" s="93"/>
-      <c r="N58" s="98">
+      <c r="L58" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="M58" s="40" t="s">
+        <v>251</v>
+      </c>
+      <c r="N58" s="9">
         <v>0.2916666666666667</v>
       </c>
       <c r="O58" s="57"/>
@@ -5260,20 +5259,20 @@
       <c r="B59" s="25"/>
       <c r="C59" s="25"/>
       <c r="D59" s="25"/>
-      <c r="E59" s="96"/>
+      <c r="E59" s="95"/>
       <c r="F59" s="25"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="25"/>
-      <c r="J59" s="97"/>
+      <c r="J59" s="96"/>
       <c r="K59" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="L59" s="93" t="s">
-        <v>223</v>
-      </c>
-      <c r="M59" s="93"/>
-      <c r="N59" s="98">
+      <c r="L59" s="90" t="s">
+        <v>160</v>
+      </c>
+      <c r="M59" s="90"/>
+      <c r="N59" s="97">
         <v>0.2916666666666667</v>
       </c>
       <c r="O59" s="57"/>
@@ -5300,22 +5299,22 @@
       <c r="B60" s="25"/>
       <c r="C60" s="25"/>
       <c r="D60" s="25"/>
-      <c r="E60" s="96"/>
+      <c r="E60" s="95"/>
       <c r="F60" s="22" t="s">
         <v>269</v>
       </c>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
-      <c r="J60" s="97"/>
-      <c r="K60" s="13" t="s">
+      <c r="J60" s="96"/>
+      <c r="K60" s="6" t="s">
         <v>270</v>
       </c>
-      <c r="L60" s="93" t="s">
+      <c r="L60" s="90" t="s">
         <v>223</v>
       </c>
-      <c r="M60" s="4"/>
-      <c r="N60" s="98">
+      <c r="M60" s="90"/>
+      <c r="N60" s="97">
         <v>0.2916666666666667</v>
       </c>
       <c r="O60" s="57"/>
@@ -5342,21 +5341,21 @@
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
-      <c r="E61" s="96"/>
+      <c r="E61" s="95"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="25"/>
-      <c r="J61" s="97"/>
+      <c r="J61" s="96"/>
       <c r="K61" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="L61" s="93" t="s">
+      <c r="L61" s="90" t="s">
         <v>223</v>
       </c>
       <c r="M61" s="4"/>
-      <c r="N61" s="9">
-        <v>0.3125</v>
+      <c r="N61" s="97">
+        <v>0.2916666666666667</v>
       </c>
       <c r="O61" s="57"/>
       <c r="P61" s="4"/>
@@ -5382,23 +5381,21 @@
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
-      <c r="E62" s="96"/>
+      <c r="E62" s="95"/>
       <c r="F62" s="25"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="25"/>
-      <c r="J62" s="97"/>
+      <c r="J62" s="96"/>
       <c r="K62" s="13" t="s">
         <v>272</v>
       </c>
-      <c r="L62" s="93" t="s">
+      <c r="L62" s="90" t="s">
         <v>223</v>
       </c>
-      <c r="M62" s="22" t="s">
-        <v>273</v>
-      </c>
+      <c r="M62" s="4"/>
       <c r="N62" s="9">
-        <v>0.2916666666666667</v>
+        <v>0.3125</v>
       </c>
       <c r="O62" s="57"/>
       <c r="P62" s="4"/>
@@ -5424,15 +5421,21 @@
       <c r="B63" s="25"/>
       <c r="C63" s="25"/>
       <c r="D63" s="25"/>
-      <c r="E63" s="96"/>
-      <c r="J63" s="97"/>
+      <c r="E63" s="95"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="96"/>
       <c r="K63" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="L63" s="90" t="s">
+        <v>223</v>
+      </c>
+      <c r="M63" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="L63" s="93" t="s">
-        <v>223</v>
-      </c>
-      <c r="M63" s="4"/>
       <c r="N63" s="9">
         <v>0.2916666666666667</v>
       </c>
@@ -5460,16 +5463,16 @@
       <c r="B64" s="25"/>
       <c r="C64" s="25"/>
       <c r="D64" s="25"/>
-      <c r="E64" s="96"/>
+      <c r="E64" s="95"/>
       <c r="F64" s="25"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="25"/>
-      <c r="J64" s="97"/>
-      <c r="K64" s="99" t="s">
+      <c r="J64" s="96"/>
+      <c r="K64" s="13" t="s">
         <v>275</v>
       </c>
-      <c r="L64" s="100" t="s">
+      <c r="L64" s="90" t="s">
         <v>223</v>
       </c>
       <c r="M64" s="4"/>
@@ -5500,16 +5503,22 @@
       <c r="B65" s="25"/>
       <c r="C65" s="25"/>
       <c r="D65" s="25"/>
-      <c r="E65" s="96"/>
+      <c r="E65" s="95"/>
       <c r="F65" s="25"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="25"/>
-      <c r="J65" s="97"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
+      <c r="J65" s="96"/>
+      <c r="K65" s="98" t="s">
+        <v>276</v>
+      </c>
+      <c r="L65" s="99" t="s">
+        <v>223</v>
+      </c>
       <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
+      <c r="N65" s="9">
+        <v>0.2916666666666667</v>
+      </c>
       <c r="O65" s="57"/>
       <c r="P65" s="4"/>
       <c r="Q65" s="4"/>
@@ -5534,15 +5543,13 @@
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
       <c r="D66" s="25"/>
-      <c r="E66" s="96"/>
+      <c r="E66" s="95"/>
       <c r="F66" s="25"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="25"/>
-      <c r="J66" s="97"/>
-      <c r="K66" s="22" t="s">
-        <v>276</v>
-      </c>
+      <c r="J66" s="96"/>
+      <c r="K66" s="22"/>
       <c r="L66" s="4"/>
       <c r="M66" s="4"/>
       <c r="N66" s="4"/>
@@ -5570,13 +5577,15 @@
       <c r="B67" s="25"/>
       <c r="C67" s="25"/>
       <c r="D67" s="25"/>
-      <c r="E67" s="96"/>
+      <c r="E67" s="95"/>
       <c r="F67" s="25"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="25"/>
-      <c r="J67" s="97"/>
-      <c r="K67" s="22"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="22" t="s">
+        <v>277</v>
+      </c>
       <c r="L67" s="4"/>
       <c r="M67" s="4"/>
       <c r="N67" s="4"/>
@@ -5604,12 +5613,12 @@
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
-      <c r="E68" s="96"/>
+      <c r="E68" s="95"/>
       <c r="F68" s="25"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="25"/>
-      <c r="J68" s="97"/>
+      <c r="J68" s="96"/>
       <c r="K68" s="22"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4"/>
@@ -5638,12 +5647,16 @@
       <c r="B69" s="25"/>
       <c r="C69" s="25"/>
       <c r="D69" s="25"/>
-      <c r="E69" s="96"/>
+      <c r="E69" s="95"/>
       <c r="F69" s="25"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="25"/>
-      <c r="J69" s="97"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="62"/>
+      <c r="L69" s="62"/>
+      <c r="M69" s="62"/>
+      <c r="N69" s="62"/>
       <c r="O69" s="57"/>
       <c r="P69" s="4"/>
       <c r="Q69" s="4"/>
@@ -5668,12 +5681,12 @@
       <c r="B70" s="25"/>
       <c r="C70" s="25"/>
       <c r="D70" s="25"/>
-      <c r="E70" s="96"/>
+      <c r="E70" s="95"/>
       <c r="F70" s="25"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="25"/>
-      <c r="J70" s="97"/>
+      <c r="J70" s="96"/>
       <c r="K70" s="22"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4"/>
@@ -5702,12 +5715,12 @@
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
       <c r="D71" s="25"/>
-      <c r="E71" s="96"/>
+      <c r="E71" s="95"/>
       <c r="F71" s="25"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="25"/>
-      <c r="J71" s="97"/>
+      <c r="J71" s="96"/>
       <c r="K71" s="22"/>
       <c r="L71" s="4"/>
       <c r="M71" s="4"/>
@@ -5736,12 +5749,12 @@
       <c r="B72" s="25"/>
       <c r="C72" s="25"/>
       <c r="D72" s="25"/>
-      <c r="E72" s="96"/>
+      <c r="E72" s="95"/>
       <c r="F72" s="25"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="25"/>
-      <c r="J72" s="97"/>
+      <c r="J72" s="96"/>
       <c r="K72" s="22"/>
       <c r="L72" s="4"/>
       <c r="M72" s="4"/>
@@ -5770,12 +5783,12 @@
       <c r="B73" s="25"/>
       <c r="C73" s="25"/>
       <c r="D73" s="25"/>
-      <c r="E73" s="96"/>
+      <c r="E73" s="95"/>
       <c r="F73" s="25"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="25"/>
-      <c r="J73" s="97"/>
+      <c r="J73" s="96"/>
       <c r="K73" s="22"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
@@ -5804,12 +5817,12 @@
       <c r="B74" s="25"/>
       <c r="C74" s="25"/>
       <c r="D74" s="25"/>
-      <c r="E74" s="96"/>
+      <c r="E74" s="95"/>
       <c r="F74" s="25"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="25"/>
-      <c r="J74" s="97"/>
+      <c r="J74" s="96"/>
       <c r="K74" s="22"/>
       <c r="L74" s="4"/>
       <c r="M74" s="4"/>
@@ -5838,12 +5851,12 @@
       <c r="B75" s="25"/>
       <c r="C75" s="25"/>
       <c r="D75" s="25"/>
-      <c r="E75" s="96"/>
+      <c r="E75" s="95"/>
       <c r="F75" s="25"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="25"/>
-      <c r="J75" s="97"/>
+      <c r="J75" s="96"/>
       <c r="K75" s="22"/>
       <c r="L75" s="4"/>
       <c r="M75" s="4"/>
@@ -5913,174 +5926,176 @@
     <hyperlink r:id="rId43" ref="P8"/>
     <hyperlink r:id="rId44" ref="A9"/>
     <hyperlink r:id="rId45" ref="F9"/>
-    <hyperlink r:id="rId46" ref="K9"/>
-    <hyperlink r:id="rId47" ref="P9"/>
-    <hyperlink r:id="rId48" ref="U9"/>
-    <hyperlink r:id="rId49" ref="A10"/>
-    <hyperlink r:id="rId50" ref="F10"/>
-    <hyperlink r:id="rId51" ref="K10"/>
-    <hyperlink r:id="rId52" ref="P10"/>
-    <hyperlink r:id="rId53" ref="U10"/>
-    <hyperlink r:id="rId54" ref="AA10"/>
-    <hyperlink r:id="rId55" ref="A11"/>
-    <hyperlink r:id="rId56" ref="F11"/>
-    <hyperlink r:id="rId57" ref="K11"/>
-    <hyperlink r:id="rId58" ref="P11"/>
-    <hyperlink r:id="rId59" ref="A12"/>
-    <hyperlink r:id="rId60" ref="F12"/>
-    <hyperlink r:id="rId61" ref="K12"/>
-    <hyperlink r:id="rId62" ref="P12"/>
-    <hyperlink r:id="rId63" ref="U12"/>
-    <hyperlink r:id="rId64" ref="F13"/>
-    <hyperlink r:id="rId65" ref="K13"/>
-    <hyperlink r:id="rId66" ref="P13"/>
-    <hyperlink r:id="rId67" ref="AA13"/>
-    <hyperlink r:id="rId68" ref="F14"/>
-    <hyperlink r:id="rId69" ref="K14"/>
-    <hyperlink r:id="rId70" ref="P14"/>
-    <hyperlink r:id="rId71" ref="F15"/>
-    <hyperlink r:id="rId72" ref="K15"/>
-    <hyperlink r:id="rId73" ref="P15"/>
-    <hyperlink r:id="rId74" ref="F16"/>
-    <hyperlink r:id="rId75" ref="K16"/>
-    <hyperlink r:id="rId76" ref="P16"/>
-    <hyperlink r:id="rId77" ref="U16"/>
-    <hyperlink r:id="rId78" ref="AA16"/>
-    <hyperlink r:id="rId79" ref="F17"/>
-    <hyperlink r:id="rId80" ref="K17"/>
-    <hyperlink r:id="rId81" ref="P17"/>
-    <hyperlink r:id="rId82" ref="U17"/>
-    <hyperlink r:id="rId83" ref="F18"/>
-    <hyperlink r:id="rId84" ref="K18"/>
-    <hyperlink r:id="rId85" ref="P18"/>
-    <hyperlink r:id="rId86" ref="U18"/>
-    <hyperlink r:id="rId87" ref="F19"/>
-    <hyperlink r:id="rId88" ref="K19"/>
-    <hyperlink r:id="rId89" ref="P19"/>
-    <hyperlink r:id="rId90" ref="U19"/>
-    <hyperlink r:id="rId91" ref="AA19"/>
-    <hyperlink r:id="rId92" ref="F20"/>
-    <hyperlink r:id="rId93" ref="K20"/>
-    <hyperlink r:id="rId94" ref="P20"/>
-    <hyperlink r:id="rId95" ref="U20"/>
-    <hyperlink r:id="rId96" ref="V20"/>
-    <hyperlink r:id="rId97" ref="F21"/>
-    <hyperlink r:id="rId98" ref="K21"/>
-    <hyperlink r:id="rId99" ref="P21"/>
-    <hyperlink r:id="rId100" ref="U21"/>
-    <hyperlink r:id="rId101" ref="F22"/>
-    <hyperlink r:id="rId102" ref="K22"/>
-    <hyperlink r:id="rId103" ref="P22"/>
-    <hyperlink r:id="rId104" ref="AA22"/>
-    <hyperlink r:id="rId105" ref="F23"/>
-    <hyperlink r:id="rId106" ref="K23"/>
-    <hyperlink r:id="rId107" ref="P23"/>
-    <hyperlink r:id="rId108" ref="F24"/>
-    <hyperlink r:id="rId109" ref="K24"/>
-    <hyperlink r:id="rId110" ref="P24"/>
-    <hyperlink r:id="rId111" ref="F25"/>
-    <hyperlink r:id="rId112" ref="K25"/>
-    <hyperlink r:id="rId113" ref="P25"/>
-    <hyperlink r:id="rId114" ref="AA25"/>
-    <hyperlink r:id="rId115" ref="F26"/>
-    <hyperlink r:id="rId116" ref="K26"/>
-    <hyperlink r:id="rId117" ref="P26"/>
-    <hyperlink r:id="rId118" ref="F27"/>
-    <hyperlink r:id="rId119" ref="K27"/>
-    <hyperlink r:id="rId120" ref="P27"/>
-    <hyperlink r:id="rId121" ref="F28"/>
-    <hyperlink r:id="rId122" ref="K28"/>
-    <hyperlink r:id="rId123" ref="P28"/>
-    <hyperlink r:id="rId124" ref="AA28"/>
-    <hyperlink r:id="rId125" ref="F29"/>
-    <hyperlink r:id="rId126" ref="K29"/>
-    <hyperlink r:id="rId127" ref="P29"/>
-    <hyperlink r:id="rId128" ref="F30"/>
-    <hyperlink r:id="rId129" ref="K30"/>
-    <hyperlink r:id="rId130" ref="P30"/>
-    <hyperlink r:id="rId131" ref="F31"/>
-    <hyperlink r:id="rId132" ref="K31"/>
-    <hyperlink r:id="rId133" ref="P31"/>
-    <hyperlink r:id="rId134" ref="AA31"/>
-    <hyperlink r:id="rId135" ref="F32"/>
-    <hyperlink r:id="rId136" ref="K32"/>
-    <hyperlink r:id="rId137" ref="P32"/>
-    <hyperlink r:id="rId138" ref="F33"/>
-    <hyperlink r:id="rId139" ref="K33"/>
-    <hyperlink r:id="rId140" ref="P33"/>
-    <hyperlink r:id="rId141" ref="F34"/>
-    <hyperlink r:id="rId142" ref="K34"/>
-    <hyperlink r:id="rId143" ref="P34"/>
-    <hyperlink r:id="rId144" ref="AA34"/>
-    <hyperlink r:id="rId145" ref="F35"/>
-    <hyperlink r:id="rId146" ref="K35"/>
-    <hyperlink r:id="rId147" ref="P35"/>
-    <hyperlink r:id="rId148" ref="F36"/>
-    <hyperlink r:id="rId149" ref="K36"/>
-    <hyperlink r:id="rId150" ref="P36"/>
-    <hyperlink r:id="rId151" ref="F37"/>
-    <hyperlink r:id="rId152" ref="K37"/>
-    <hyperlink r:id="rId153" ref="P37"/>
-    <hyperlink r:id="rId154" ref="AA37"/>
-    <hyperlink r:id="rId155" ref="F38"/>
-    <hyperlink r:id="rId156" ref="K38"/>
-    <hyperlink r:id="rId157" ref="P38"/>
-    <hyperlink r:id="rId158" ref="F39"/>
-    <hyperlink r:id="rId159" ref="K39"/>
-    <hyperlink r:id="rId160" ref="P39"/>
-    <hyperlink r:id="rId161" ref="F40"/>
-    <hyperlink r:id="rId162" ref="K40"/>
-    <hyperlink r:id="rId163" ref="P40"/>
-    <hyperlink r:id="rId164" ref="AA40"/>
-    <hyperlink r:id="rId165" ref="F41"/>
-    <hyperlink r:id="rId166" ref="K41"/>
-    <hyperlink r:id="rId167" ref="P41"/>
-    <hyperlink r:id="rId168" ref="F42"/>
-    <hyperlink r:id="rId169" ref="K42"/>
-    <hyperlink r:id="rId170" ref="F43"/>
-    <hyperlink r:id="rId171" ref="K43"/>
-    <hyperlink r:id="rId172" ref="AA43"/>
-    <hyperlink r:id="rId173" ref="F44"/>
-    <hyperlink r:id="rId174" ref="K44"/>
-    <hyperlink r:id="rId175" ref="F45"/>
-    <hyperlink r:id="rId176" ref="K45"/>
-    <hyperlink r:id="rId177" ref="F46"/>
-    <hyperlink r:id="rId178" ref="K46"/>
-    <hyperlink r:id="rId179" ref="AA46"/>
-    <hyperlink r:id="rId180" ref="F47"/>
-    <hyperlink r:id="rId181" ref="K47"/>
-    <hyperlink r:id="rId182" ref="F48"/>
-    <hyperlink r:id="rId183" ref="K48"/>
-    <hyperlink r:id="rId184" ref="F49"/>
-    <hyperlink r:id="rId185" ref="K49"/>
-    <hyperlink r:id="rId186" ref="AA49"/>
-    <hyperlink r:id="rId187" ref="F50"/>
-    <hyperlink r:id="rId188" ref="K50"/>
-    <hyperlink r:id="rId189" ref="F51"/>
-    <hyperlink r:id="rId190" ref="K51"/>
-    <hyperlink r:id="rId191" ref="F52"/>
-    <hyperlink r:id="rId192" ref="K52"/>
-    <hyperlink r:id="rId193" ref="AA52"/>
-    <hyperlink r:id="rId194" ref="F53"/>
-    <hyperlink r:id="rId195" ref="K53"/>
-    <hyperlink r:id="rId196" ref="F54"/>
-    <hyperlink r:id="rId197" ref="K54"/>
-    <hyperlink r:id="rId198" ref="F55"/>
-    <hyperlink r:id="rId199" ref="K55"/>
-    <hyperlink r:id="rId200" ref="F56"/>
-    <hyperlink r:id="rId201" ref="K56"/>
-    <hyperlink r:id="rId202" ref="F57"/>
-    <hyperlink r:id="rId203" ref="K57"/>
-    <hyperlink r:id="rId204" ref="F58"/>
-    <hyperlink r:id="rId205" ref="K58"/>
-    <hyperlink r:id="rId206" ref="K59"/>
-    <hyperlink r:id="rId207" ref="K60"/>
-    <hyperlink r:id="rId208" ref="K61"/>
-    <hyperlink r:id="rId209" ref="K62"/>
-    <hyperlink r:id="rId210" ref="K63"/>
-    <hyperlink r:id="rId211" ref="K64"/>
+    <hyperlink r:id="rId46" ref="H9"/>
+    <hyperlink r:id="rId47" ref="K9"/>
+    <hyperlink r:id="rId48" ref="P9"/>
+    <hyperlink r:id="rId49" ref="U9"/>
+    <hyperlink r:id="rId50" ref="A10"/>
+    <hyperlink r:id="rId51" ref="F10"/>
+    <hyperlink r:id="rId52" ref="K10"/>
+    <hyperlink r:id="rId53" ref="P10"/>
+    <hyperlink r:id="rId54" ref="U10"/>
+    <hyperlink r:id="rId55" ref="AA10"/>
+    <hyperlink r:id="rId56" ref="A11"/>
+    <hyperlink r:id="rId57" ref="F11"/>
+    <hyperlink r:id="rId58" ref="K11"/>
+    <hyperlink r:id="rId59" ref="P11"/>
+    <hyperlink r:id="rId60" ref="A12"/>
+    <hyperlink r:id="rId61" ref="F12"/>
+    <hyperlink r:id="rId62" ref="K12"/>
+    <hyperlink r:id="rId63" ref="P12"/>
+    <hyperlink r:id="rId64" ref="U12"/>
+    <hyperlink r:id="rId65" ref="F13"/>
+    <hyperlink r:id="rId66" ref="K13"/>
+    <hyperlink r:id="rId67" ref="P13"/>
+    <hyperlink r:id="rId68" ref="AA13"/>
+    <hyperlink r:id="rId69" ref="F14"/>
+    <hyperlink r:id="rId70" ref="K14"/>
+    <hyperlink r:id="rId71" ref="P14"/>
+    <hyperlink r:id="rId72" ref="F15"/>
+    <hyperlink r:id="rId73" ref="K15"/>
+    <hyperlink r:id="rId74" ref="P15"/>
+    <hyperlink r:id="rId75" ref="F16"/>
+    <hyperlink r:id="rId76" ref="K16"/>
+    <hyperlink r:id="rId77" ref="P16"/>
+    <hyperlink r:id="rId78" ref="U16"/>
+    <hyperlink r:id="rId79" ref="AA16"/>
+    <hyperlink r:id="rId80" ref="F17"/>
+    <hyperlink r:id="rId81" ref="K17"/>
+    <hyperlink r:id="rId82" ref="P17"/>
+    <hyperlink r:id="rId83" ref="U17"/>
+    <hyperlink r:id="rId84" ref="F18"/>
+    <hyperlink r:id="rId85" ref="K18"/>
+    <hyperlink r:id="rId86" ref="P18"/>
+    <hyperlink r:id="rId87" ref="U18"/>
+    <hyperlink r:id="rId88" ref="F19"/>
+    <hyperlink r:id="rId89" ref="K19"/>
+    <hyperlink r:id="rId90" ref="P19"/>
+    <hyperlink r:id="rId91" ref="U19"/>
+    <hyperlink r:id="rId92" ref="AA19"/>
+    <hyperlink r:id="rId93" ref="F20"/>
+    <hyperlink r:id="rId94" ref="K20"/>
+    <hyperlink r:id="rId95" ref="P20"/>
+    <hyperlink r:id="rId96" ref="U20"/>
+    <hyperlink r:id="rId97" ref="V20"/>
+    <hyperlink r:id="rId98" ref="F21"/>
+    <hyperlink r:id="rId99" ref="K21"/>
+    <hyperlink r:id="rId100" ref="P21"/>
+    <hyperlink r:id="rId101" ref="U21"/>
+    <hyperlink r:id="rId102" ref="F22"/>
+    <hyperlink r:id="rId103" ref="K22"/>
+    <hyperlink r:id="rId104" ref="P22"/>
+    <hyperlink r:id="rId105" ref="AA22"/>
+    <hyperlink r:id="rId106" ref="F23"/>
+    <hyperlink r:id="rId107" ref="K23"/>
+    <hyperlink r:id="rId108" ref="P23"/>
+    <hyperlink r:id="rId109" ref="F24"/>
+    <hyperlink r:id="rId110" ref="K24"/>
+    <hyperlink r:id="rId111" ref="P24"/>
+    <hyperlink r:id="rId112" ref="F25"/>
+    <hyperlink r:id="rId113" ref="K25"/>
+    <hyperlink r:id="rId114" ref="P25"/>
+    <hyperlink r:id="rId115" ref="AA25"/>
+    <hyperlink r:id="rId116" ref="F26"/>
+    <hyperlink r:id="rId117" ref="K26"/>
+    <hyperlink r:id="rId118" ref="P26"/>
+    <hyperlink r:id="rId119" ref="F27"/>
+    <hyperlink r:id="rId120" ref="K27"/>
+    <hyperlink r:id="rId121" ref="P27"/>
+    <hyperlink r:id="rId122" ref="F28"/>
+    <hyperlink r:id="rId123" ref="K28"/>
+    <hyperlink r:id="rId124" ref="P28"/>
+    <hyperlink r:id="rId125" ref="AA28"/>
+    <hyperlink r:id="rId126" ref="F29"/>
+    <hyperlink r:id="rId127" ref="K29"/>
+    <hyperlink r:id="rId128" ref="P29"/>
+    <hyperlink r:id="rId129" ref="F30"/>
+    <hyperlink r:id="rId130" ref="K30"/>
+    <hyperlink r:id="rId131" ref="P30"/>
+    <hyperlink r:id="rId132" ref="F31"/>
+    <hyperlink r:id="rId133" ref="K31"/>
+    <hyperlink r:id="rId134" ref="P31"/>
+    <hyperlink r:id="rId135" ref="AA31"/>
+    <hyperlink r:id="rId136" ref="F32"/>
+    <hyperlink r:id="rId137" ref="K32"/>
+    <hyperlink r:id="rId138" ref="P32"/>
+    <hyperlink r:id="rId139" ref="F33"/>
+    <hyperlink r:id="rId140" ref="K33"/>
+    <hyperlink r:id="rId141" ref="P33"/>
+    <hyperlink r:id="rId142" ref="F34"/>
+    <hyperlink r:id="rId143" ref="K34"/>
+    <hyperlink r:id="rId144" ref="P34"/>
+    <hyperlink r:id="rId145" ref="AA34"/>
+    <hyperlink r:id="rId146" ref="F35"/>
+    <hyperlink r:id="rId147" ref="K35"/>
+    <hyperlink r:id="rId148" ref="P35"/>
+    <hyperlink r:id="rId149" ref="F36"/>
+    <hyperlink r:id="rId150" ref="K36"/>
+    <hyperlink r:id="rId151" ref="P36"/>
+    <hyperlink r:id="rId152" ref="F37"/>
+    <hyperlink r:id="rId153" ref="K37"/>
+    <hyperlink r:id="rId154" ref="P37"/>
+    <hyperlink r:id="rId155" ref="AA37"/>
+    <hyperlink r:id="rId156" ref="F38"/>
+    <hyperlink r:id="rId157" ref="K38"/>
+    <hyperlink r:id="rId158" ref="P38"/>
+    <hyperlink r:id="rId159" ref="F39"/>
+    <hyperlink r:id="rId160" ref="K39"/>
+    <hyperlink r:id="rId161" ref="P39"/>
+    <hyperlink r:id="rId162" ref="F40"/>
+    <hyperlink r:id="rId163" ref="K40"/>
+    <hyperlink r:id="rId164" ref="P40"/>
+    <hyperlink r:id="rId165" ref="AA40"/>
+    <hyperlink r:id="rId166" ref="F41"/>
+    <hyperlink r:id="rId167" ref="K41"/>
+    <hyperlink r:id="rId168" ref="P41"/>
+    <hyperlink r:id="rId169" ref="F42"/>
+    <hyperlink r:id="rId170" ref="K42"/>
+    <hyperlink r:id="rId171" ref="F43"/>
+    <hyperlink r:id="rId172" ref="K43"/>
+    <hyperlink r:id="rId173" ref="AA43"/>
+    <hyperlink r:id="rId174" ref="F44"/>
+    <hyperlink r:id="rId175" ref="K44"/>
+    <hyperlink r:id="rId176" ref="F45"/>
+    <hyperlink r:id="rId177" ref="K45"/>
+    <hyperlink r:id="rId178" ref="F46"/>
+    <hyperlink r:id="rId179" ref="K46"/>
+    <hyperlink r:id="rId180" ref="AA46"/>
+    <hyperlink r:id="rId181" ref="F47"/>
+    <hyperlink r:id="rId182" ref="K47"/>
+    <hyperlink r:id="rId183" ref="F48"/>
+    <hyperlink r:id="rId184" ref="K48"/>
+    <hyperlink r:id="rId185" ref="F49"/>
+    <hyperlink r:id="rId186" ref="K49"/>
+    <hyperlink r:id="rId187" ref="AA49"/>
+    <hyperlink r:id="rId188" ref="F50"/>
+    <hyperlink r:id="rId189" ref="K50"/>
+    <hyperlink r:id="rId190" ref="F51"/>
+    <hyperlink r:id="rId191" ref="K51"/>
+    <hyperlink r:id="rId192" ref="F52"/>
+    <hyperlink r:id="rId193" ref="K52"/>
+    <hyperlink r:id="rId194" ref="AA52"/>
+    <hyperlink r:id="rId195" ref="F53"/>
+    <hyperlink r:id="rId196" ref="K53"/>
+    <hyperlink r:id="rId197" ref="F54"/>
+    <hyperlink r:id="rId198" ref="K54"/>
+    <hyperlink r:id="rId199" ref="F55"/>
+    <hyperlink r:id="rId200" ref="K55"/>
+    <hyperlink r:id="rId201" ref="F56"/>
+    <hyperlink r:id="rId202" ref="K56"/>
+    <hyperlink r:id="rId203" ref="F57"/>
+    <hyperlink r:id="rId204" ref="K57"/>
+    <hyperlink r:id="rId205" ref="F58"/>
+    <hyperlink r:id="rId206" ref="K58"/>
+    <hyperlink r:id="rId207" ref="K59"/>
+    <hyperlink r:id="rId208" ref="K60"/>
+    <hyperlink r:id="rId209" ref="K61"/>
+    <hyperlink r:id="rId210" ref="K62"/>
+    <hyperlink r:id="rId211" ref="K63"/>
+    <hyperlink r:id="rId212" ref="K64"/>
+    <hyperlink r:id="rId213" ref="K65"/>
   </hyperlinks>
-  <drawing r:id="rId212"/>
-  <legacyDrawing r:id="rId213"/>
+  <drawing r:id="rId214"/>
+  <legacyDrawing r:id="rId215"/>
 </worksheet>
 </file>
</xml_diff>